<commit_message>
Funciona bien el login
</commit_message>
<xml_diff>
--- a/st-parranderos-jdo-est/docs/It1_C-02_df.serrano_ms.alvarezl - Modelo Relacional.xlsx
+++ b/st-parranderos-jdo-est/docs/It1_C-02_df.serrano_ms.alvarezl - Modelo Relacional.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/ms_alvarezl_uniandes_edu_co/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sofiaalvarez/Desktop/It2_C-02_ms-alvarezl_df.serrano/st-parranderos-jdo-est/st-parranderos-jdo-est/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1041" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{E49D186B-A6C8-4955-8FF2-A5E1631EB615}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FF1725-F79A-E54B-8F7C-CBCAA369F3F2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="147">
   <si>
     <t>Usuarios</t>
   </si>
@@ -420,6 +420,54 @@
   </si>
   <si>
     <t>idConsumo</t>
+  </si>
+  <si>
+    <t>Convenciones</t>
+  </si>
+  <si>
+    <t>idConvencion</t>
+  </si>
+  <si>
+    <t>fechaInicio</t>
+  </si>
+  <si>
+    <t>fechaFin</t>
+  </si>
+  <si>
+    <t>idUsuario</t>
+  </si>
+  <si>
+    <t>NN, CK &gt;= 0</t>
+  </si>
+  <si>
+    <t>CK (después del 2019 y después de fechaInicio)</t>
+  </si>
+  <si>
+    <t>FK(Usuario.numDocumento)</t>
+  </si>
+  <si>
+    <t>FK(Planes.idPlan)</t>
+  </si>
+  <si>
+    <t>FK (Convencion.idConvencion), Nullable</t>
+  </si>
+  <si>
+    <t>Mantenimientos</t>
+  </si>
+  <si>
+    <t>idMantenimiento</t>
+  </si>
+  <si>
+    <t>causa</t>
+  </si>
+  <si>
+    <t>numHabitacion</t>
+  </si>
+  <si>
+    <t>FK (Horario.idHorario)</t>
+  </si>
+  <si>
+    <t>FK (Habitaciones.numeroHabitacion), Nullable</t>
   </si>
 </sst>
 </file>
@@ -435,7 +483,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -484,8 +532,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -602,15 +662,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -628,11 +679,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -695,64 +805,115 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1069,48 +1230,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:P50"/>
+  <dimension ref="A2:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" customWidth="1"/>
-    <col min="5" max="5" width="33.140625" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" customWidth="1"/>
-    <col min="8" max="8" width="33.42578125" customWidth="1"/>
-    <col min="9" max="9" width="47.85546875" customWidth="1"/>
-    <col min="10" max="10" width="54.42578125" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="28.42578125" customWidth="1"/>
-    <col min="13" max="13" width="25.42578125" customWidth="1"/>
-    <col min="14" max="14" width="29.28515625" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" customWidth="1"/>
-    <col min="16" max="16" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="37.1640625" customWidth="1"/>
+    <col min="4" max="4" width="34.5" customWidth="1"/>
+    <col min="5" max="5" width="33.1640625" customWidth="1"/>
+    <col min="6" max="6" width="37" customWidth="1"/>
+    <col min="7" max="7" width="34.5" customWidth="1"/>
+    <col min="8" max="8" width="33.5" customWidth="1"/>
+    <col min="9" max="9" width="47.83203125" customWidth="1"/>
+    <col min="10" max="10" width="54.5" customWidth="1"/>
+    <col min="11" max="11" width="30.6640625" customWidth="1"/>
+    <col min="12" max="12" width="31.83203125" customWidth="1"/>
+    <col min="13" max="13" width="25.5" customWidth="1"/>
+    <col min="14" max="14" width="29.33203125" customWidth="1"/>
+    <col min="15" max="15" width="34.6640625" customWidth="1"/>
+    <col min="16" max="16" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="34" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="35"/>
+      <c r="J2" s="33"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1123,10 +1284,10 @@
       <c r="E3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="37"/>
+      <c r="G3" s="44"/>
       <c r="H3" s="3"/>
       <c r="I3" s="11" t="s">
         <v>6</v>
@@ -1136,7 +1297,7 @@
       </c>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1149,10 +1310,10 @@
       <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="37"/>
+      <c r="G4" s="44"/>
       <c r="H4" s="3"/>
       <c r="I4" s="11" t="s">
         <v>13</v>
@@ -1162,58 +1323,61 @@
       </c>
       <c r="K4" s="3"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="49"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="J7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="M7" s="9" t="s">
+      <c r="M7" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="N7" s="9" t="s">
+      <c r="N7" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="O7" s="12"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O7" s="55" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="E8" s="11" t="s">
@@ -1243,29 +1407,31 @@
       <c r="M8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="N8" s="9" t="s">
+      <c r="N8" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="12"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="O8" s="28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="36" t="s">
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
@@ -1300,7 +1466,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>8</v>
       </c>
@@ -1335,31 +1501,31 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="38" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B14" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="38"/>
+      <c r="C14" s="32"/>
       <c r="D14" s="15"/>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="40"/>
-      <c r="I14" s="33" t="s">
+      <c r="F14" s="36"/>
+      <c r="I14" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="33"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" s="14" t="s">
         <v>55</v>
       </c>
@@ -1382,14 +1548,14 @@
       <c r="K15" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="L15" s="37" t="s">
+      <c r="L15" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="M15" s="37"/>
+      <c r="M15" s="44"/>
       <c r="N15" s="3"/>
       <c r="O15" s="6"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" s="17" t="s">
         <v>8</v>
       </c>
@@ -1412,35 +1578,35 @@
       <c r="K16" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="L16" s="37" t="s">
+      <c r="L16" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="37"/>
+      <c r="M16" s="44"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G17" s="13"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="35" t="s">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B19" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="40" t="s">
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="42"/>
-      <c r="L19" s="42"/>
-      <c r="O19" s="41"/>
-      <c r="P19" s="41"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="O19" s="35"/>
+      <c r="P19" s="35"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B20" s="21" t="s">
         <v>69</v>
       </c>
@@ -1477,7 +1643,7 @@
       <c r="O20" s="16"/>
       <c r="P20" s="16"/>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B21" s="14" t="s">
         <v>10</v>
       </c>
@@ -1514,27 +1680,27 @@
       <c r="O21" s="16"/>
       <c r="P21" s="16"/>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="30" t="s">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B23" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="32"/>
-      <c r="J23" s="29" t="s">
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="41"/>
+      <c r="J23" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="K23" s="29"/>
+      <c r="K23" s="38"/>
       <c r="L23" s="15"/>
       <c r="M23" s="15"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>84</v>
       </c>
@@ -1565,10 +1731,10 @@
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
       <c r="N24" s="12"/>
-      <c r="O24" s="43"/>
-      <c r="P24" s="43"/>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25" s="11" t="s">
         <v>8</v>
       </c>
@@ -1599,44 +1765,48 @@
       <c r="L25" s="12"/>
       <c r="M25" s="12"/>
       <c r="N25" s="12"/>
-      <c r="O25" s="43"/>
-      <c r="P25" s="43"/>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="46" t="s">
+      <c r="O25" s="30"/>
+      <c r="P25" s="30"/>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B27" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="H27" s="33" t="s">
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
-      <c r="N27" s="33"/>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="42"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B28" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="F28" s="28" t="s">
+      <c r="F28" s="55" t="s">
         <v>130</v>
       </c>
-      <c r="H28" s="23" t="s">
+      <c r="G28" s="59" t="s">
+        <v>132</v>
+      </c>
+      <c r="H28" s="56" t="s">
         <v>95</v>
       </c>
       <c r="I28" s="5" t="s">
@@ -1658,7 +1828,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B29" s="11" t="s">
         <v>100</v>
       </c>
@@ -1674,7 +1844,10 @@
       <c r="F29" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="H29" s="7" t="s">
+      <c r="G29" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="H29" s="57" t="s">
         <v>8</v>
       </c>
       <c r="I29" s="11" t="s">
@@ -1696,21 +1869,22 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="45" t="s">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B31" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="45"/>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="64"/>
+      <c r="H31" s="64"/>
+      <c r="I31" s="64"/>
+      <c r="J31" s="64"/>
+      <c r="K31" s="64"/>
+      <c r="L31" s="65"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B32" s="5" t="s">
         <v>105</v>
       </c>
@@ -1738,11 +1912,14 @@
       <c r="J32" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="K32" s="23" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L32" s="46" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B33" s="11" t="s">
         <v>100</v>
       </c>
@@ -1770,81 +1947,82 @@
       <c r="J33" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="K33" s="11" t="s">
+      <c r="K33" s="7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="38" t="s">
+      <c r="L33" s="46" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B36" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="48"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="11" t="s">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B37" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="F37" s="11" t="s">
-        <v>4</v>
-      </c>
+      <c r="F37" s="29"/>
       <c r="G37" s="10"/>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="11" t="s">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B38" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E38" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F38" s="11" t="s">
-        <v>44</v>
-      </c>
+      <c r="F38" s="29"/>
       <c r="G38" s="10"/>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B40" s="35" t="s">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B40" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="3"/>
-      <c r="G40" s="44" t="s">
+      <c r="C40" s="47"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="47"/>
+      <c r="G40" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="H40" s="44"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="11" t="s">
+      <c r="H40" s="34"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="34"/>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B41" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="E41" s="10"/>
+      <c r="E41" s="46" t="s">
+        <v>36</v>
+      </c>
       <c r="G41" s="11" t="s">
         <v>122</v>
       </c>
@@ -1858,17 +2036,19 @@
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="11" t="s">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B42" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="E42" s="10"/>
+      <c r="E42" s="46" t="s">
+        <v>10</v>
+      </c>
       <c r="G42" s="11" t="s">
         <v>8</v>
       </c>
@@ -1882,13 +2062,13 @@
         <v>124</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="34" t="s">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B44" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="C44" s="34"/>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C44" s="31"/>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B45" s="11" t="s">
         <v>40</v>
       </c>
@@ -1896,7 +2076,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B46" s="11" t="s">
         <v>117</v>
       </c>
@@ -1904,15 +2084,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="34" t="s">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B48" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="C48" s="34"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B49" s="11" t="s">
         <v>127</v>
       </c>
@@ -1926,7 +2106,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B50" s="11" t="s">
         <v>8</v>
       </c>
@@ -1940,22 +2120,113 @@
         <v>129</v>
       </c>
     </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B52" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="C52" s="50"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="50"/>
+      <c r="G52" s="50"/>
+      <c r="H52" s="50"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B53" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C53" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E53" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="F53" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="G53" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="H53" s="28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B54" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="E54" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="F54" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="G54" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="H54" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B56" s="66" t="s">
+        <v>141</v>
+      </c>
+      <c r="C56" s="66"/>
+      <c r="D56" s="66"/>
+      <c r="E56" s="66"/>
+      <c r="F56" s="66"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B57" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="C57" s="52" t="s">
+        <v>143</v>
+      </c>
+      <c r="D57" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="E57" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="F57" s="52" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B58" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="52" t="s">
+        <v>145</v>
+      </c>
+      <c r="E58" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="F58" s="52" t="s">
+        <v>146</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="G40:J40"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="H19:L19"/>
-    <mergeCell ref="E6:N6"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="A10:E10"/>
+  <mergeCells count="29">
+    <mergeCell ref="B52:H52"/>
+    <mergeCell ref="E6:O6"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="B56:F56"/>
     <mergeCell ref="J23:K23"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="H27:N27"/>
@@ -1969,6 +2240,17 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="E14:F14"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="H19:L19"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="G40:J40"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B36:E36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>